<commit_message>
add excel and image compose&paste demo
</commit_message>
<xml_diff>
--- a/01-python/01-test/a.xlsx
+++ b/01-python/01-test/a.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2832" yWindow="936" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -28,14 +27,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -59,15 +65,102 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12192000" cy="4876800"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12192000" cy="4876800"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12192000" cy="4876800"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,18 +447,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="n">
@@ -376,7 +469,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>43905.9413799</v>
       </c>
     </row>
@@ -398,5 +491,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>